<commit_message>
if an image has already been parsed, it won't be again
</commit_message>
<xml_diff>
--- a/Projeto PConc.xlsx
+++ b/Projeto PConc.xlsx
@@ -1,20 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E214C-1FA9-485E-8591-EC03EAF70DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Dataset 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Dataset 2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Dataset 3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Dataset 4" sheetId="4" r:id="rId7"/>
+    <sheet name="Dataset 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dataset 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Dataset 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Dataset 4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
   <si>
     <t>Execution Time</t>
   </si>
@@ -57,23 +79,50 @@
   <si>
     <t>Laptop</t>
   </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Asus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i7-10875H </t>
+  </si>
+  <si>
+    <t>2.30 GHz</t>
+  </si>
+  <si>
+    <t>16Gb</t>
+  </si>
+  <si>
+    <t>WSL</t>
+  </si>
+  <si>
+    <t>/WSL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00_);(#,##0.00)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -83,41 +132,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -134,7 +198,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -147,9 +211,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -179,18 +245,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Dataset 1'!$A$3:$A$8</c:f>
-            </c:strRef>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 1'!$B$3:$B$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.31</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-747C-4146-8E62-57E1DFA26D28}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 1'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 1'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DA09-491D-8E20-B17CB7709F67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1312834318"/>
         <c:axId val="1869238267"/>
       </c:lineChart>
@@ -198,7 +389,7 @@
         <c:axId val="1312834318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -217,7 +408,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -233,7 +424,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -246,9 +437,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869238267"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1869238267"/>
@@ -292,7 +489,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -324,9 +521,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1312834318"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -344,16 +544,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -370,7 +582,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -383,9 +595,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -414,19 +628,90 @@
               </a:ln>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Dataset 1'!$F$3:$F$8</c:f>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 1'!$G$3:$G$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00_);\(#\ ##0.00\)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7852564102564104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3601694915254239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2958579881656807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8680555555555558</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2519083969465647</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F2BB-45AB-9395-548289A8EDC6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Asus</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 1'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD2D-4734-857B-E5014D7AFA25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="561668115"/>
         <c:axId val="561718572"/>
       </c:lineChart>
@@ -434,7 +719,7 @@
         <c:axId val="561668115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -453,7 +738,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -469,7 +754,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -482,9 +767,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="561718572"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="561718572"/>
@@ -528,7 +819,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -541,7 +832,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00_);\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -560,9 +851,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="561668115"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -580,16 +874,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -606,7 +912,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -619,9 +925,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -651,18 +959,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'Dataset 2'!$A$3:$A$8</c:f>
-            </c:strRef>
+            <c:numRef>
+              <c:f>'Dataset 2'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 2'!$B$3:$B$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>21.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.44</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBD5-45DF-883E-ECD3535F8F46}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 2'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 2'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB18-4F57-A3AB-AD288B059E8E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="643699355"/>
         <c:axId val="125728850"/>
       </c:lineChart>
@@ -670,7 +1103,7 @@
         <c:axId val="643699355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -689,7 +1122,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -705,7 +1138,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -718,9 +1151,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="125728850"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="125728850"/>
@@ -764,7 +1203,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -796,9 +1235,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="643699355"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -816,16 +1258,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -842,7 +1296,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -855,9 +1309,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -887,18 +1343,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Dataset 2'!$F$3:$F$8</c:f>
-            </c:strRef>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 2'!$G$3:$G$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00_);\(#\ ##0.00\)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7454110135674383</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5759717314487633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3036253776435047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0276243093922659</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0202205882352944</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D82-454F-8FB1-40BC5356F417}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 2'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 2'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9AF6-47BB-AD32-BD9E9C4E36D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1327994248"/>
         <c:axId val="676032701"/>
       </c:lineChart>
@@ -906,7 +1487,7 @@
         <c:axId val="1327994248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -925,7 +1506,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -941,7 +1522,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -954,9 +1535,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="676032701"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="676032701"/>
@@ -1000,7 +1587,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1013,7 +1600,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00_);\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1032,9 +1619,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1327994248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1052,16 +1642,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1078,7 +1680,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -1091,9 +1693,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1123,18 +1727,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'Dataset 3'!$A$3:$A$8</c:f>
-            </c:strRef>
+            <c:numRef>
+              <c:f>'Dataset 3'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 3'!$B$3:$B$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F7A-4FAB-9775-87A2C595E77B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 3'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 3'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>77.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.032</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F982-463F-9A85-888B0FB05116}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="3038505"/>
         <c:axId val="130896600"/>
       </c:lineChart>
@@ -1142,7 +1871,7 @@
         <c:axId val="3038505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1161,7 +1890,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1177,7 +1906,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1190,9 +1919,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="130896600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="130896600"/>
@@ -1236,7 +1971,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1268,9 +2003,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="3038505"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1288,16 +2026,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1314,7 +2064,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -1327,9 +2077,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1358,19 +2110,90 @@
               </a:ln>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Dataset 3'!$F$3:$F$8</c:f>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 3'!$G$3:$G$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00_);\(#\ ##0.00\)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4546728971962617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3565480696442087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1928205128205129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4665924276169262</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4208791208791207</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B22-44A5-A0AD-79838FB4DA71}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 3'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3561-4F7C-9556-B0818D2361ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1582442989"/>
         <c:axId val="599660990"/>
       </c:lineChart>
@@ -1378,7 +2201,7 @@
         <c:axId val="1582442989"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1397,7 +2220,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1413,7 +2236,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1426,9 +2249,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="599660990"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="599660990"/>
@@ -1472,7 +2301,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1485,7 +2314,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00_);\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1504,9 +2333,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1582442989"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1524,16 +2356,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1550,7 +2394,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -1563,9 +2407,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1595,18 +2441,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'Dataset 4'!$A$3:$A$8</c:f>
-            </c:strRef>
+            <c:numRef>
+              <c:f>'Dataset 4'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 4'!$B$3:$B$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>37.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.98</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3CD2-44D3-87E2-E3D1713965DA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 4'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 4'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>77.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-775F-4546-A6EB-ACA92C33312C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="363870522"/>
         <c:axId val="977226392"/>
       </c:lineChart>
@@ -1614,7 +2585,7 @@
         <c:axId val="363870522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1633,7 +2604,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1649,7 +2620,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1662,9 +2633,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="977226392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="977226392"/>
@@ -1708,7 +2685,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1740,9 +2717,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="363870522"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1760,16 +2740,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1786,7 +2778,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-PT" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -1799,9 +2791,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1831,18 +2825,143 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Dataset 4'!$F$3:$F$8</c:f>
-            </c:strRef>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Dataset 4'!$G$3:$G$8</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00_);\(#\ ##0.00\)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0649985619787172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8019464720194647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8095599393019728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9102428722280886</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1236080178173715</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-415F-4E7A-9D66-0B49834D4B4D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ASUS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dataset 4'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dataset 4'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C91-4037-BDFE-805DD200B73D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1982420270"/>
         <c:axId val="1729330251"/>
       </c:lineChart>
@@ -1850,7 +2969,7 @@
         <c:axId val="1982420270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1869,7 +2988,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1885,7 +3004,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1898,9 +3017,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1729330251"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1729330251"/>
@@ -1944,7 +3069,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="pt-PT" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1957,7 +3082,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00_);\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1976,9 +3101,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1982420270"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1996,16 +3124,24 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2014,9 +3150,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2025,7 +3167,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2039,9 +3181,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2050,7 +3198,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2060,7 +3208,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2069,9 +3217,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2080,7 +3234,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2094,9 +3248,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2105,7 +3265,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2115,7 +3275,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2124,9 +3284,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2135,7 +3301,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2149,9 +3315,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2160,7 +3332,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2170,7 +3342,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2179,9 +3351,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2190,7 +3368,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2204,9 +3382,15 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2215,7 +3399,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2225,7 +3409,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2415,24 +3599,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.25"/>
-    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2441,223 +3630,283 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>5.57</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="1">
+        <v>10.86</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="1">$B$3/$B3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="0">$B$3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>3.12</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="4">
+        <v>6.65</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>1.78525641</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7852564102564104</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.63</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>2.36</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="1"/>
-        <v>2.360169492</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3601694915254239</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.04</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>1.69</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="1"/>
-        <v>3.295857988</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2958579881656807</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.33</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>1.44</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="1"/>
-        <v>3.868055556</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8680555555555558</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2.91</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>1.31</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="1">
+        <v>3.62</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="1"/>
-        <v>4.251908397</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="14">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2519083969465647</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2666,223 +3915,278 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>21.87</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="1">
+        <v>45.7</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="1">$B$3/$B3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="0">$B$3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>45.7/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>12.53</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="4">
+        <v>28.18</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>1.745411014</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7454110135674383</v>
+      </c>
+      <c r="H4">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>8.49</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="1">
+        <v>20.77</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="1"/>
-        <v>2.575971731</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5759717314487633</v>
+      </c>
+      <c r="H5">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>6.62</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="1">
+        <v>17.18</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="1"/>
-        <v>3.303625378</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3036253776435047</v>
+      </c>
+      <c r="H6">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>5.43</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="1">
+        <v>16.89</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="1"/>
-        <v>4.027624309</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0276243093922659</v>
+      </c>
+      <c r="H7">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>5.44</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="1">
+        <v>17.28</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="1"/>
-        <v>4.020220588</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="14">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0202205882352944</v>
+      </c>
+      <c r="H8">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2891,223 +4195,279 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>31.13</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="1">
+        <v>77.47</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="1">$B$3/$B3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="0">$B$3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <f>77.47/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>21.4</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="4">
+        <v>48.79</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>1.454672897</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4546728971962617</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>13.21</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="1">
+        <v>33.25</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="1"/>
-        <v>2.35654807</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3565480696442087</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>9.75</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="1">
+        <v>27.02</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="1"/>
-        <v>3.192820513</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1928205128205129</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>8.98</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="1">
+        <v>23.99</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="1"/>
-        <v>3.466592428</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4665924276169262</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>9.1</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="1">
+        <v>23.032</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="1"/>
-        <v>3.420879121</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="14">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4208791208791207</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3116,208 +4476,261 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>37.03</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="1">
+        <v>77.69</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="1">$B$3/$B3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="0">$B$3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>77.69/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>34.77</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+        <v>34.770000000000003</v>
+      </c>
+      <c r="C4" s="4">
+        <v>72.41</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>1.064998562</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0649985619787172</v>
+      </c>
+      <c r="H4">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>20.55</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="1">
+        <v>46.23</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="1"/>
-        <v>1.801946472</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8019464720194647</v>
+      </c>
+      <c r="H5">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>13.18</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="1"/>
-        <v>2.809559939</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8095599393019728</v>
+      </c>
+      <c r="H6">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>9.47</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="C7" s="1">
+        <v>27.67</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="1"/>
-        <v>3.910242872</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9102428722280886</v>
+      </c>
+      <c r="H7">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>8.98</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="1">
+        <v>24.99</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="1"/>
-        <v>4.123608018</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="14">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1236080178173715</v>
+      </c>
+      <c r="H8">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>